<commit_message>
Updated VSP Test Cases to include thread.sleep
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/VSP-Data.xlsx
+++ b/KatalonData/Bootstrap/VSP-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KatalonData\Bootstrap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t465179\Documents\git\VPS-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CBC2D4-4679-4458-80B7-FC72DE44F616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC0465B-95C4-48F9-8922-B63C158E82C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="893" firstSheet="2" activeTab="11" xr2:uid="{F85E046C-D3FC-46F9-AA2F-5165245A7308}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="893" firstSheet="6" activeTab="11" xr2:uid="{F85E046C-D3FC-46F9-AA2F-5165245A7308}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateProfile" sheetId="1" r:id="rId1"/>
@@ -468,9 +468,6 @@
     <t>This Profile has been modified</t>
   </si>
   <si>
-    <t>2025</t>
-  </si>
-  <si>
     <t>ExpMonthCCMod</t>
   </si>
   <si>
@@ -688,6 +685,9 @@
   </si>
   <si>
     <t>imtiazstergosh@gmail.com</t>
+  </si>
+  <si>
+    <t>2029</t>
   </si>
 </sst>
 </file>
@@ -744,13 +744,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -769,9 +768,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -809,7 +808,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -915,7 +914,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1057,7 +1056,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1071,40 +1070,40 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="24.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="26" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="32" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="16384" width="24.28515625" style="1"/>
+    <col min="20" max="20" width="6.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="12.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="25.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="16384" width="24.26953125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1208,7 +1207,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="C2" s="1" t="s">
         <v>42</v>
       </c>
@@ -1237,7 +1236,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
       <c r="C3" s="1" t="s">
         <v>43</v>
       </c>
@@ -1289,7 +1288,7 @@
       <c r="T3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="W3" t="s">
         <v>54</v>
       </c>
       <c r="X3" s="1" t="s">
@@ -1330,6 +1329,9 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1337,44 +1339,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F32B79-CCE8-401C-87BF-7A6DD5C015A7}">
   <dimension ref="A1:AL5"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AI2" sqref="AI2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="24.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.54296875" style="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30" style="1" customWidth="1"/>
-    <col min="9" max="9" width="23.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.453125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1796875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.81640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="6.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.81640625" style="1" customWidth="1"/>
     <col min="17" max="17" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="26" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="32" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="31.42578125" style="1" customWidth="1"/>
-    <col min="35" max="16384" width="24.28515625" style="1"/>
+    <col min="20" max="20" width="6.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="12.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="31.453125" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="24.26953125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1490,9 +1492,9 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.35">
       <c r="C2" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -1510,19 +1512,19 @@
         <v>12</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>51</v>
@@ -1533,7 +1535,7 @@
       <c r="S2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="W2" t="s">
         <v>54</v>
       </c>
       <c r="X2" s="1" t="s">
@@ -1567,13 +1569,13 @@
         <v>61</v>
       </c>
       <c r="AH2" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="AI2" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="AJ2" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="AK2" s="1" t="s">
         <v>102</v>
@@ -1582,9 +1584,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.35">
       <c r="C3" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
@@ -1602,19 +1604,19 @@
         <v>12</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L3" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>51</v>
@@ -1625,7 +1627,7 @@
       <c r="S3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="W3" t="s">
         <v>54</v>
       </c>
       <c r="X3" s="1" t="s">
@@ -1659,10 +1661,10 @@
         <v>61</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AI3" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AJ3" s="1" t="s">
         <v>83</v>
@@ -1674,9 +1676,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.35">
       <c r="C4" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
@@ -1694,19 +1696,19 @@
         <v>12</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>51</v>
@@ -1717,7 +1719,7 @@
       <c r="S4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="W4" s="2" t="s">
+      <c r="W4" t="s">
         <v>54</v>
       </c>
       <c r="X4" s="1" t="s">
@@ -1751,10 +1753,10 @@
         <v>61</v>
       </c>
       <c r="AH4" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AI4" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AJ4" s="1" t="s">
         <v>91</v>
@@ -1766,9 +1768,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.35">
       <c r="C5" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>8</v>
@@ -1786,19 +1788,19 @@
         <v>12</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L5" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>51</v>
@@ -1809,7 +1811,7 @@
       <c r="S5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="W5" s="2" t="s">
+      <c r="W5" t="s">
         <v>54</v>
       </c>
       <c r="X5" s="1" t="s">
@@ -1843,10 +1845,10 @@
         <v>61</v>
       </c>
       <c r="AH5" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AI5" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AJ5" s="1" t="s">
         <v>101</v>
@@ -1860,6 +1862,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1871,40 +1876,40 @@
       <selection activeCell="AM1" sqref="AM1:AM1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="24.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.54296875" style="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.81640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.26953125" style="1" customWidth="1"/>
     <col min="17" max="17" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="26" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="32" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="33.85546875" style="1" customWidth="1"/>
-    <col min="35" max="16384" width="24.28515625" style="1"/>
+    <col min="20" max="20" width="6.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="12.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="33.81640625" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="24.26953125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2008,21 +2013,21 @@
         <v>38</v>
       </c>
       <c r="AI1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="AL1" s="1" t="s">
-        <v>148</v>
-      </c>
     </row>
-    <row r="2" spans="1:38" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" ht="29" x14ac:dyDescent="0.35">
       <c r="C2" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -2040,19 +2045,19 @@
         <v>12</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>51</v>
@@ -2063,7 +2068,7 @@
       <c r="S2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="W2" s="2" t="s">
         <v>54</v>
       </c>
       <c r="X2" s="1" t="s">
@@ -2097,24 +2102,24 @@
         <v>61</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AJ2" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AK2" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" ht="29" x14ac:dyDescent="0.35">
       <c r="C3" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
@@ -2132,19 +2137,19 @@
         <v>12</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L3" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>51</v>
@@ -2155,7 +2160,7 @@
       <c r="S3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="W3" s="2" t="s">
         <v>54</v>
       </c>
       <c r="X3" s="1" t="s">
@@ -2189,24 +2194,24 @@
         <v>61</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AI3" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AJ3" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AK3" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AL3" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
-    <row r="4" spans="1:38" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.35">
       <c r="C4" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
@@ -2224,19 +2229,19 @@
         <v>12</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>51</v>
@@ -2247,7 +2252,7 @@
       <c r="S4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="W4" s="2" t="s">
         <v>54</v>
       </c>
       <c r="X4" s="1" t="s">
@@ -2281,24 +2286,27 @@
         <v>61</v>
       </c>
       <c r="AH4" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AI4" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="AJ4" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="AK4" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AL4" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2310,22 +2318,22 @@
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="24.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30" style="1" customWidth="1"/>
-    <col min="9" max="9" width="32.5703125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="31.5703125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="24.28515625" style="1"/>
+    <col min="9" max="9" width="32.54296875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="31.54296875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="24.26953125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2357,7 +2365,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
@@ -2374,13 +2382,13 @@
         <v>12</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
@@ -2397,13 +2405,13 @@
         <v>12</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
@@ -2420,13 +2428,13 @@
         <v>12</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
@@ -2443,13 +2451,13 @@
         <v>12</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
@@ -2466,13 +2474,13 @@
         <v>12</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
@@ -2489,13 +2497,13 @@
         <v>12</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D8" s="1" t="s">
         <v>8</v>
       </c>
@@ -2512,13 +2520,13 @@
         <v>12</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
@@ -2534,16 +2542,19 @@
       <c r="H9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>213</v>
+      <c r="I9" t="s">
+        <v>212</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2555,22 +2566,22 @@
       <selection activeCell="I1" sqref="I1:J1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1" bestFit="1"/>
-    <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="1" bestFit="1"/>
+    <col min="6" max="6" width="24.453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30" style="1" customWidth="1"/>
     <col min="9" max="9" width="23" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="17.81640625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2602,7 +2613,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C2" s="1" t="s">
         <v>42</v>
       </c>
@@ -2631,6 +2642,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2642,40 +2656,40 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1" bestFit="1"/>
-    <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="1" bestFit="1"/>
+    <col min="6" max="6" width="24.453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="26" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="32" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="16384" width="9.140625" style="1"/>
+    <col min="20" max="20" width="6.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="12.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="25.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2779,7 +2793,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
@@ -2808,6 +2822,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2815,44 +2832,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94B1EDA5-E3A3-4794-9389-11A1BB516C67}">
   <dimension ref="A1:AU3"/>
   <sheetViews>
-    <sheetView topLeftCell="AP1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AV1" sqref="AV1:AW1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="24.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.54296875" style="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="26" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="32" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="16384" width="24.28515625" style="1"/>
+    <col min="20" max="20" width="6.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="12.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="25.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="16384" width="24.26953125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2995,7 +3012,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
       <c r="C2" s="1" t="s">
         <v>94</v>
       </c>
@@ -3063,7 +3080,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
       <c r="C3" s="1" t="s">
         <v>95</v>
       </c>
@@ -3118,6 +3135,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -3125,44 +3145,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC310AF0-6FFB-4A8E-A2F9-ECD1411C076E}">
   <dimension ref="A1:AL2"/>
   <sheetViews>
-    <sheetView topLeftCell="AD1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AD1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="24.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.54296875" style="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="26" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="32" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="16384" width="24.28515625" style="1"/>
+    <col min="20" max="20" width="6.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="12.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="25.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="16384" width="24.26953125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3278,7 +3298,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.35">
       <c r="C2" s="1" t="s">
         <v>95</v>
       </c>
@@ -3330,7 +3350,7 @@
       <c r="T2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="W2" t="s">
         <v>54</v>
       </c>
       <c r="X2" s="1" t="s">
@@ -3381,6 +3401,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -3388,44 +3411,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4940B053-892E-4D65-970C-387445E934F5}">
   <dimension ref="A1:AX2"/>
   <sheetViews>
-    <sheetView topLeftCell="AE1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AS1" sqref="AS1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="24.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="29" style="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.5703125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.1796875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.54296875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="6.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="26" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="32" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="16384" width="24.28515625" style="1"/>
+    <col min="20" max="20" width="6.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="12.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="25.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="16384" width="24.26953125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3577,7 +3600,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:50" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" ht="29" x14ac:dyDescent="0.35">
       <c r="C2" s="1" t="s">
         <v>43</v>
       </c>
@@ -3629,7 +3652,7 @@
       <c r="T2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="W2" t="s">
         <v>54</v>
       </c>
       <c r="X2" s="1" t="s">
@@ -3698,7 +3721,7 @@
       <c r="AS2" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="AT2" s="2" t="s">
+      <c r="AT2" t="s">
         <v>135</v>
       </c>
       <c r="AU2" s="1" t="s">
@@ -3716,6 +3739,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -3723,44 +3749,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4C6E2C-C42D-471F-A066-CEBAB5BA432C}">
   <dimension ref="A1:AN2"/>
   <sheetViews>
-    <sheetView topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AA1" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AN2" sqref="AN2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="24.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.54296875" style="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="26" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="32" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="16384" width="24.28515625" style="1"/>
+    <col min="20" max="20" width="6.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="12.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="25.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="16384" width="24.26953125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3876,13 +3902,13 @@
         <v>74</v>
       </c>
       <c r="AM1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="AN1" s="1" t="s">
-        <v>142</v>
-      </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
       <c r="C2" s="1" t="s">
         <v>95</v>
       </c>
@@ -3934,7 +3960,7 @@
       <c r="T2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="W2" t="s">
         <v>54</v>
       </c>
       <c r="X2" s="1" t="s">
@@ -3980,17 +4006,20 @@
         <v>102</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>140</v>
+        <v>85</v>
       </c>
       <c r="AM2" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AN2" s="1" t="s">
-        <v>85</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -3998,44 +4027,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD29F020-32F0-46BA-9C78-0D5D38002911}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="1"/>
+    <col min="6" max="6" width="24.453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="26" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="32" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="16384" width="9.140625" style="1"/>
+    <col min="20" max="20" width="6.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="12.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="25.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4139,7 +4168,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
@@ -4167,6 +4196,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -4174,44 +4206,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{055BC8D0-1CFC-40D6-9313-A3584BAD2B30}">
   <dimension ref="A1:AM4"/>
   <sheetViews>
-    <sheetView topLeftCell="Y1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Y1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="24.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.54296875" style="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="26" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="32" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="16384" width="24.28515625" style="1"/>
+    <col min="20" max="20" width="6.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="12.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="25.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="16384" width="24.26953125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4315,24 +4347,24 @@
         <v>38</v>
       </c>
       <c r="AI1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="AL1" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="AM1" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.35">
       <c r="C2" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -4382,7 +4414,7 @@
       <c r="T2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="W2" t="s">
         <v>54</v>
       </c>
       <c r="X2" s="1" t="s">
@@ -4416,27 +4448,27 @@
         <v>61</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AJ2" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK2" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="AK2" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="AL2" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AM2" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.35">
       <c r="C3" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
@@ -4486,7 +4518,7 @@
       <c r="T3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="W3" t="s">
         <v>54</v>
       </c>
       <c r="X3" s="1" t="s">
@@ -4520,27 +4552,27 @@
         <v>61</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AI3" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AJ3" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AK3" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL3" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AM3" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.35">
       <c r="C4" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
@@ -4590,7 +4622,7 @@
       <c r="T4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="W4" s="2" t="s">
+      <c r="W4" t="s">
         <v>54</v>
       </c>
       <c r="X4" s="1" t="s">
@@ -4624,25 +4656,28 @@
         <v>61</v>
       </c>
       <c r="AH4" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AI4" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="AJ4" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="AK4" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AL4" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AM4" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>